<commit_message>
Complete !!! version 1.0
</commit_message>
<xml_diff>
--- a/build/classes/db/RoomStock.xlsx
+++ b/build/classes/db/RoomStock.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t>Premium</t>
+  </si>
+  <si>
+    <t>24-04-2020 03:28:54</t>
+  </si>
+  <si>
+    <t>24-04-2020 03:30:52</t>
+  </si>
+  <si>
+    <t>24-04-2020 03:31:01</t>
+  </si>
+  <si>
+    <t>24-04-2020 03:33:59</t>
+  </si>
+  <si>
+    <t>24-04-2020 03:34:24</t>
+  </si>
+  <si>
+    <t>24-04-2020 03:35:03</t>
   </si>
 </sst>
 </file>
@@ -128,7 +146,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1800,66 +1818,194 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2061.0</v>
+        <v>2052.0</v>
       </c>
       <c r="B53" t="n">
-        <v>8005.0</v>
+        <v>1200.0</v>
       </c>
       <c r="C53" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
       </c>
       <c r="F53" t="n">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="G53" t="n">
         <v>1.0</v>
       </c>
       <c r="H53" t="n">
-        <v>7500.0</v>
+        <v>1200.0</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
       </c>
       <c r="J53" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2062.0</v>
+        <v>2053.0</v>
       </c>
       <c r="B54" t="n">
-        <v>8006.0</v>
+        <v>1200.0</v>
       </c>
       <c r="C54" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D54" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E54" t="s">
         <v>12</v>
       </c>
       <c r="F54" t="n">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="G54" t="n">
         <v>1.0</v>
       </c>
       <c r="H54" t="n">
-        <v>7500.0</v>
+        <v>1200.0</v>
       </c>
       <c r="I54" t="s">
         <v>13</v>
       </c>
       <c r="J54" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2054.0</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1300.0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H55" t="n">
+        <v>1300.0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>13</v>
+      </c>
+      <c r="J55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>2055.0</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1102.0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H56" t="n">
+        <v>1102.0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>13</v>
+      </c>
+      <c r="J56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>2056.0</v>
+      </c>
+      <c r="B57" t="n">
+        <v>9999.0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>9999.0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>13</v>
+      </c>
+      <c r="J57" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>2057.0</v>
+      </c>
+      <c r="B58" t="n">
+        <v>9999.0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H58" t="n">
+        <v>9999.0</v>
+      </c>
+      <c r="I58" t="s">
+        <v>13</v>
+      </c>
+      <c r="J58" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>